<commit_message>
tambah bukti evaluasi kesesuaian peresepan thd forpus EP07
</commit_message>
<xml_diff>
--- a/ukp/3.10_Kefarmasian/EP 07/Lap Evaluasi Peresepan.xlsx
+++ b/ukp/3.10_Kefarmasian/EP 07/Lap Evaluasi Peresepan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7875"/>
+    <workbookView windowWidth="20490" windowHeight="7875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="JANUARI 2024" sheetId="9" r:id="rId1"/>
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
-  <si>
-    <t>LAPORAN PEMANTAUAN PENULISAN RESEP OBAT GENERIK DI PUSKESMAS DAN JARINGANNYA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
+  <si>
+    <t>LAPORAN PEMANTAUAN PENULISAN RESEP OBAT TERHADAP FORPUS</t>
   </si>
   <si>
     <t>Puskesmas : BERAKIT</t>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t xml:space="preserve"> NIP. 19891012 202203 1 001</t>
-  </si>
-  <si>
-    <t>LAPORAN EVALUASI PENULISAN RESEP OBAT  DI PUSKESMAS DAN JARINGANNYA</t>
   </si>
   <si>
     <t>Februari</t>
@@ -128,11 +125,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[$-409]d/mmm"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-409]d/mmm"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -187,46 +184,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,8 +199,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -256,6 +254,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -263,9 +285,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,52 +327,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -346,49 +343,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,7 +511,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,121 +523,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,15 +565,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -588,6 +576,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,17 +604,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,22 +639,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,148 +667,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -844,20 +841,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -954,6 +951,363 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>470535</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>77470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1292225</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="ttd_mentor-removebg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="958850" y="5135245"/>
+          <a:ext cx="821690" cy="878205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1341755</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>138430</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="ttd-arif"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6985635" y="2609850"/>
+          <a:ext cx="4136390" cy="5461635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>673735</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>705485</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>86995</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="cappkm-removebg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1162050" y="3150870"/>
+          <a:ext cx="3752215" cy="4946650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1369695</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>90805</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>154940</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>157480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="ttd-arif"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7013575" y="2624455"/>
+          <a:ext cx="4124960" cy="5543550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>77470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1356360</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>128270</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="ttd_mentor-removebg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028065" y="5135245"/>
+          <a:ext cx="816610" cy="860425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>483870</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>572770</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>58420</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="cappkm-removebg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="972185" y="3041650"/>
+          <a:ext cx="3809365" cy="5027295"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1464945</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>250190</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="ttd-arif"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7108825" y="2583180"/>
+          <a:ext cx="4124960" cy="5543550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>281305</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>50165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1097915</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="ttd_mentor-removebg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="769620" y="5107940"/>
+          <a:ext cx="816610" cy="860425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>483870</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85090</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="cappkm-removebg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="972185" y="2960370"/>
+          <a:ext cx="3760470" cy="4973320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1216,8 +1570,8 @@
   <sheetPr/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:F10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75"/>
@@ -1666,9 +2020,10 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C9"/>
   </mergeCells>
-  <pageMargins left="1.57013888888889" right="0.390277777777778" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="1.22013888888889" right="0.390277777777778" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1678,7 +2033,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:F10"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75"/>
@@ -1695,7 +2050,7 @@
   <sheetData>
     <row r="1" ht="18" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1737,7 +2092,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" ht="14.25" spans="1:7">
@@ -2038,7 +2393,7 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -2127,9 +2482,10 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C9"/>
   </mergeCells>
-  <pageMargins left="1.57013888888889" right="0.390277777777778" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="1.02361111111111" right="0.390277777777778" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2138,8 +2494,8 @@
   <sheetPr/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:F10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75"/>
@@ -2156,7 +2512,7 @@
   <sheetData>
     <row r="1" ht="18" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2198,7 +2554,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" ht="14.25" spans="1:7">
@@ -2499,7 +2855,7 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -2588,8 +2944,9 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C9"/>
   </mergeCells>
-  <pageMargins left="1.57013888888889" right="0.390277777777778" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="1.10208333333333" right="0.390277777777778" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>